<commit_message>
Atualização da planilha de perguntas e respostas
</commit_message>
<xml_diff>
--- a/cartas_e_matriz_gabarito_game_of_selects.xlsx
+++ b/cartas_e_matriz_gabarito_game_of_selects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Desktop\game-of-selects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\Arquivos SP Tech\Banco de Dados\game-of-selects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F46002D-32C5-49A2-8869-0E8E3A5080CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99329E4-2096-41BB-9FB9-121121D5E52D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{9311D172-BD3F-4CF1-B3BB-28AA954A7D86}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="cartas.xlsx" sheetId="1" r:id="rId1"/>
     <sheet name="matriz" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,10 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="26">
   <si>
     <t>Conteúdo do Select</t>
   </si>
@@ -220,6 +217,12 @@
   </si>
   <si>
     <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Exibir os nomes das seleções, os nomes de seus respectivos jogadores, o número da camisa e a posição em que cada um joga</t>
+  </si>
+  <si>
+    <t>SELECT selecao.pais AS 'Seleção', jogador.nome AS 'Jogador', jogador.numeroCamisa AS 'Camisa', jogador.posicao AS 'Posição' FROM selecao JOIN jogador ON jogador.fkSelecao = selecao.idSelecao;</t>
   </si>
 </sst>
 </file>
@@ -294,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -367,17 +370,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -401,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -411,7 +403,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,11 +411,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -452,7 +442,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,6 +459,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,8 +531,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8782050" y="1190625"/>
+          <a:off x="6753225" y="1190625"/>
           <a:ext cx="1409897" cy="809738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3276600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1932102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CB2B410-1256-4F94-8E61-6775C099FA76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6753225" y="5629275"/>
+          <a:ext cx="3200400" cy="1865427"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -839,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC23502-0A7C-4E91-A919-706747D674F7}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,737 +901,737 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="50.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
+      <c r="A2" s="22">
         <v>99</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="25"/>
+      <c r="F2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>99</v>
-      </c>
-      <c r="B3" s="18">
+        <v>10</v>
+      </c>
+      <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="18" t="s">
+      <c r="C3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="23" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>99</v>
-      </c>
-      <c r="B4" s="18">
+        <v>10</v>
+      </c>
+      <c r="B4" s="16">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="8"/>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7"/>
       <c r="F4" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>99</v>
-      </c>
-      <c r="B5" s="18">
+        <v>10</v>
+      </c>
+      <c r="B5" s="16">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="8"/>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7"/>
       <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>99</v>
-      </c>
-      <c r="B6" s="18">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="8"/>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7"/>
       <c r="F6" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>99</v>
-      </c>
-      <c r="B7" s="18">
+        <v>10</v>
+      </c>
+      <c r="B7" s="16">
         <v>5</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="8"/>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7"/>
       <c r="F7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>99</v>
-      </c>
-      <c r="B8" s="18">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="B8" s="16">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7"/>
       <c r="F8" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>99</v>
-      </c>
-      <c r="B9" s="18">
+        <v>10</v>
+      </c>
+      <c r="B9" s="16">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="8"/>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7"/>
       <c r="F9" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>99</v>
-      </c>
-      <c r="B10" s="18">
+        <v>10</v>
+      </c>
+      <c r="B10" s="16">
         <v>8</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="8"/>
+      <c r="C10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7"/>
       <c r="F10" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>99</v>
-      </c>
-      <c r="B11" s="18">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="8"/>
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="7"/>
       <c r="F11" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>99</v>
-      </c>
-      <c r="B12" s="10">
-        <v>10</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="10" t="s">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="22" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>99</v>
-      </c>
-      <c r="B13" s="18">
+        <v>10</v>
+      </c>
+      <c r="B13" s="16">
         <v>11</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="8"/>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="7"/>
       <c r="F13" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>99</v>
-      </c>
-      <c r="B14" s="18">
+        <v>10</v>
+      </c>
+      <c r="B14" s="16">
         <v>12</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="8"/>
+      <c r="C14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="7"/>
       <c r="F14" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>99</v>
-      </c>
-      <c r="B15" s="18">
+        <v>10</v>
+      </c>
+      <c r="B15" s="16">
         <v>13</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="8"/>
+      <c r="C15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="7"/>
       <c r="F15" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>99</v>
-      </c>
-      <c r="B16" s="18">
-        <v>14</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="B16" s="16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7"/>
       <c r="F16" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>99</v>
-      </c>
-      <c r="B17" s="10">
+      <c r="A17" s="4">
+        <v>10</v>
+      </c>
+      <c r="B17" s="8">
         <v>15</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="10" t="s">
+      <c r="C17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>99</v>
-      </c>
-      <c r="B18" s="18">
+      <c r="G17" s="8"/>
+      <c r="H17" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="33" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28">
+        <v>10</v>
+      </c>
+      <c r="B18" s="29">
         <v>16</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="6" t="s">
+      <c r="C18" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="21" t="s">
+      <c r="G18" s="32"/>
+      <c r="H18" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>99</v>
-      </c>
-      <c r="B19" s="18">
+        <v>10</v>
+      </c>
+      <c r="B19" s="16">
         <v>17</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="8"/>
+      <c r="C19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="7"/>
       <c r="F19" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>99</v>
-      </c>
-      <c r="B20" s="18">
+        <v>10</v>
+      </c>
+      <c r="B20" s="16">
         <v>18</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="8"/>
+      <c r="C20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="7"/>
       <c r="F20" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>99</v>
-      </c>
-      <c r="B21" s="18">
+        <v>10</v>
+      </c>
+      <c r="B21" s="16">
         <v>19</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="8"/>
+      <c r="C21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="7"/>
       <c r="F21" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>99</v>
-      </c>
-      <c r="B22" s="18">
+        <v>10</v>
+      </c>
+      <c r="B22" s="16">
         <v>20</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="8"/>
+      <c r="C22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="7"/>
       <c r="F22" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>99</v>
-      </c>
-      <c r="B23" s="18">
+        <v>10</v>
+      </c>
+      <c r="B23" s="16">
         <v>21</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="8"/>
+      <c r="C23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="7"/>
       <c r="F23" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>99</v>
-      </c>
-      <c r="B24" s="18">
+        <v>10</v>
+      </c>
+      <c r="B24" s="16">
         <v>22</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="8"/>
+      <c r="C24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="7"/>
       <c r="F24" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>99</v>
-      </c>
-      <c r="B25" s="18">
+        <v>10</v>
+      </c>
+      <c r="B25" s="16">
         <v>23</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="8"/>
+      <c r="C25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="7"/>
       <c r="F25" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>99</v>
-      </c>
-      <c r="B26" s="18">
+        <v>10</v>
+      </c>
+      <c r="B26" s="16">
         <v>24</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="8"/>
+      <c r="C26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="7"/>
       <c r="F26" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="23" t="s">
+      <c r="H26" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>99</v>
-      </c>
-      <c r="B27" s="10">
+      <c r="A27" s="4">
+        <v>10</v>
+      </c>
+      <c r="B27" s="8">
         <v>25</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="10" t="s">
+      <c r="C27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="22" t="s">
+      <c r="G27" s="8"/>
+      <c r="H27" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>99</v>
-      </c>
-      <c r="B28" s="18">
+      <c r="A28" s="4">
+        <v>10</v>
+      </c>
+      <c r="B28" s="16">
         <v>26</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="6" t="s">
+      <c r="C28" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="21" t="s">
+      <c r="G28" s="5"/>
+      <c r="H28" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>99</v>
-      </c>
-      <c r="B29" s="18">
+        <v>10</v>
+      </c>
+      <c r="B29" s="16">
         <v>27</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="8"/>
+      <c r="C29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="7"/>
       <c r="F29" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="23" t="s">
+      <c r="H29" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>99</v>
-      </c>
-      <c r="B30" s="18">
+        <v>10</v>
+      </c>
+      <c r="B30" s="16">
         <v>28</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="8"/>
+      <c r="C30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="7"/>
       <c r="F30" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="H30" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>99</v>
-      </c>
-      <c r="B31" s="18">
+        <v>10</v>
+      </c>
+      <c r="B31" s="16">
         <v>29</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="8"/>
+      <c r="C31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="7"/>
       <c r="F31" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="23" t="s">
+      <c r="H31" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>99</v>
-      </c>
-      <c r="B32" s="10">
+        <v>10</v>
+      </c>
+      <c r="B32" s="8">
         <v>30</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="8"/>
+      <c r="C32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="7"/>
       <c r="F32" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="23" t="s">
+      <c r="H32" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>99</v>
-      </c>
-      <c r="B33" s="18">
+      <c r="A33" s="4">
+        <v>10</v>
+      </c>
+      <c r="B33" s="16">
         <v>31</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="6" t="s">
+      <c r="C33" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="21" t="s">
+      <c r="G33" s="5"/>
+      <c r="H33" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
-        <v>99</v>
-      </c>
-      <c r="B34" s="10">
+      <c r="A34" s="4">
+        <v>10</v>
+      </c>
+      <c r="B34" s="8">
         <v>32</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="10" t="s">
+      <c r="C34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="22" t="s">
+      <c r="G34" s="8"/>
+      <c r="H34" s="20" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completando questões facéis e algumas questões médias
</commit_message>
<xml_diff>
--- a/cartas_e_matriz_gabarito_game_of_selects.xlsx
+++ b/cartas_e_matriz_gabarito_game_of_selects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\Arquivos SP Tech\Banco de Dados\game-of-selects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wallace\game-of-selects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99329E4-2096-41BB-9FB9-121121D5E52D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9836890C-757F-40EC-B0B1-DD959B360465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{9311D172-BD3F-4CF1-B3BB-28AA954A7D86}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="58">
   <si>
     <t>Conteúdo do Select</t>
   </si>
@@ -223,6 +223,110 @@
   </si>
   <si>
     <t>SELECT selecao.pais AS 'Seleção', jogador.nome AS 'Jogador', jogador.numeroCamisa AS 'Camisa', jogador.posicao AS 'Posição' FROM selecao JOIN jogador ON jogador.fkSelecao = selecao.idSelecao;</t>
+  </si>
+  <si>
+    <t>Exiba os nomes dos jogadores que começam com a letra L</t>
+  </si>
+  <si>
+    <t>select * from jogador 
+ where nome like "l%";</t>
+  </si>
+  <si>
+    <t>select qtdJogos, qtdDerrotas, golsPros, qtdJogos from classificacao order by qtdJogos, qtdDerrotas, golsPros, qtdJogos asc;</t>
+  </si>
+  <si>
+    <t>Exibir apenas os jogos, derrotas os gols, as quantidades de jogos da classificação em ordem crescente</t>
+  </si>
+  <si>
+    <t>Exibir apenas os países que terminam com i</t>
+  </si>
+  <si>
+    <t>select pais from selecao
+ where pais like "%i";</t>
+  </si>
+  <si>
+    <t>Exiba as selecões</t>
+  </si>
+  <si>
+    <t>Exibir as selecões que tenham técnico que começam com T</t>
+  </si>
+  <si>
+    <t>select * from selecao
+ where tecnico like "t%";</t>
+  </si>
+  <si>
+    <t>Exiba os jogadores</t>
+  </si>
+  <si>
+    <t>select * from jogador;</t>
+  </si>
+  <si>
+    <t>select * from selecao;</t>
+  </si>
+  <si>
+    <t>Exiba os estádios</t>
+  </si>
+  <si>
+    <t>select * from estádio;</t>
+  </si>
+  <si>
+    <t>Exibir apenas os nomes dos estádios em ordem alfabetica</t>
+  </si>
+  <si>
+    <t>select nome from estadio order by nome asc;</t>
+  </si>
+  <si>
+    <t>Exiba a arbitragem</t>
+  </si>
+  <si>
+    <t>select * from arbitragem;</t>
+  </si>
+  <si>
+    <t>Exibir apenas o nome do arbitro e do bandeirinha1 que começam com m</t>
+  </si>
+  <si>
+    <t>select nomeArbitroOficial, nomeBandeirinha1 from arbitragem
+ where nomeArbitroOficial like "m%" and nomeBandeirinha1 like "m%";</t>
+  </si>
+  <si>
+    <t>Exibir apenas o arbitro que se chama Ma Ning</t>
+  </si>
+  <si>
+    <t>select nomeArbitroOficial from arbitragem where nomeArbitroOficial = 'Ma Ning';</t>
+  </si>
+  <si>
+    <t>Exibir os jogadores que são lateral-esquerdo</t>
+  </si>
+  <si>
+    <t>select * from jogador
+ where posicao = 'lateral-esquerdo';</t>
+  </si>
+  <si>
+    <t>Exibir os jogadores pela camisa em ordem decrescente</t>
+  </si>
+  <si>
+    <t>select * from jogador order by numeroCamisa desc;</t>
+  </si>
+  <si>
+    <t>Exibir apenas os jogadores que são camisa 10</t>
+  </si>
+  <si>
+    <t>select * from jogador
+ where numeroCamisa = '10';</t>
+  </si>
+  <si>
+    <t>select * from selecao
+where pais like "%s";</t>
+  </si>
+  <si>
+    <t>Exibir os paises que terminam com s</t>
+  </si>
+  <si>
+    <t>Exibir as seleções os seus gols e suas vitorias, derrotas e seus jogos</t>
+  </si>
+  <si>
+    <t>select golsPros, qtdVitorias, qtdDerrotas, qtdJogos, selecao.* from selecao
+ join classificacao on selecao.idSelecao = fkSelecao;etc</t>
   </si>
 </sst>
 </file>
@@ -393,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -433,9 +537,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -477,6 +578,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,6 +696,806 @@
         <a:xfrm>
           <a:off x="6753225" y="5629275"/>
           <a:ext cx="3200400" cy="1865427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2124075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>869622</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1234347F-77D4-4161-B048-853FADFC6503}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6753225" y="2038350"/>
+          <a:ext cx="2047875" cy="850572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3371849</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1438274</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>923253</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4278649-B91A-4CE1-87D9-8F2294926D31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6677024" y="2905125"/>
+          <a:ext cx="1438275" cy="913728"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>800209</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>371524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1F6AA09-D876-4109-9577-347AAC757171}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6696075" y="3867150"/>
+          <a:ext cx="781159" cy="352474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1439307</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>876300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F599C53A-C9CF-41DC-868D-3EAF85D387FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6657976" y="4238626"/>
+          <a:ext cx="1420256" cy="866774"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1743318</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>495369</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagem 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84099EBC-AD8C-4E57-BA98-8F06D24A8E8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="5162550"/>
+          <a:ext cx="1743318" cy="495369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3181794</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>638264</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagem 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D74892DE-2008-4267-9928-CF840AF11DB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="5667375"/>
+          <a:ext cx="3181794" cy="638264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3362325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>676275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>833534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagem 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03E9E603-1848-416C-9BEA-B12503B0B70D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6629400" y="6343650"/>
+          <a:ext cx="1600200" cy="843059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>818228</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagem 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA85E2EB-24EF-41CC-B1D2-EBC0A5E71720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="7219950"/>
+          <a:ext cx="990600" cy="799178"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3504498</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1104900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagem 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29371AA9-5A30-4671-AB29-A91015288252}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="8029575"/>
+          <a:ext cx="3504498" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2953162</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>362001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Imagem 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66E9B03D-5462-4298-B645-3A4C7BE4E4B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="9172575"/>
+          <a:ext cx="2953162" cy="362001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1228895</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>352473</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Imagem 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A1A393-576D-4864-961E-75460DDE8D22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648450" y="9944100"/>
+          <a:ext cx="1219370" cy="342948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2028825</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>851477</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagem 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3D3273C-7670-4E1D-BF8B-1D9F85ED2AA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="10315576"/>
+          <a:ext cx="2028825" cy="851476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1837413</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Imagem 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8EE4097-A142-4FD1-8633-0E870E1EDC27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638926" y="11191875"/>
+          <a:ext cx="1837412" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2524125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Imagem 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBD8A30D-BF23-4DA3-A5E4-3EEB503A7790}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="11982450"/>
+          <a:ext cx="2524125" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1981200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4469</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Imagem 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9EABA6E-AB5B-4823-AB44-60542B5BB3C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="12820650"/>
+          <a:ext cx="1981200" cy="709319"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2752725</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>835557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Imagem 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E533603-5ECD-43C3-A4A7-82D027C09A57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="15592425"/>
+          <a:ext cx="2752725" cy="835557"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -891,13 +1810,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC23502-0A7C-4E91-A919-706747D674F7}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="50.5703125" style="3" customWidth="1"/>
@@ -934,24 +1853,24 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+      <c r="A2" s="21">
         <v>99</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -962,43 +1881,43 @@
       <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="18"/>
+      <c r="C3" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="17"/>
       <c r="F3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="16"/>
-      <c r="H3" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>10</v>
       </c>
       <c r="B4" s="16">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
+      <c r="C4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>10</v>
       </c>
@@ -1006,62 +1925,61 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>10</v>
       </c>
       <c r="B6" s="16">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7"/>
+      <c r="C6" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>37</v>
+      </c>
       <c r="F6" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>10</v>
       </c>
       <c r="B7" s="16">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>6</v>
+      <c r="C7" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>10</v>
       </c>
@@ -1069,105 +1987,105 @@
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>10</v>
       </c>
       <c r="B9" s="16">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>6</v>
+      <c r="C9" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>39</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>10</v>
       </c>
       <c r="B10" s="16">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>6</v>
+      <c r="C10" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>41</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="16">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>6</v>
+      <c r="C11" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>43</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>6</v>
+      <c r="C12" s="38" t="s">
+        <v>44</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="8"/>
-      <c r="H12" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10</v>
       </c>
@@ -1175,62 +2093,62 @@
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>6</v>
+        <v>46</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>10</v>
       </c>
       <c r="B14" s="16">
         <v>12</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>6</v>
+      <c r="C14" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>49</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>10</v>
       </c>
       <c r="B15" s="16">
         <v>13</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>6</v>
+      <c r="C15" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>10</v>
       </c>
@@ -1238,20 +2156,20 @@
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>6</v>
+        <v>52</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>10</v>
       </c>
@@ -1259,43 +2177,43 @@
         <v>15</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="8"/>
-      <c r="H17" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="33" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
-        <v>10</v>
-      </c>
-      <c r="B18" s="29">
+      <c r="H17" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="32" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>10</v>
+      </c>
+      <c r="B18" s="28">
         <v>16</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32" t="s">
+      <c r="E18" s="30"/>
+      <c r="F18" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="31"/>
+      <c r="H18" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>10</v>
       </c>
@@ -1303,16 +2221,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1333,7 +2251,7 @@
       <c r="F20" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1354,7 +2272,7 @@
       <c r="F21" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1375,7 +2293,7 @@
       <c r="F22" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1396,7 +2314,7 @@
       <c r="F23" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1417,7 +2335,7 @@
       <c r="F24" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1438,7 +2356,7 @@
       <c r="F25" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1459,7 +2377,7 @@
       <c r="F26" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1481,7 +2399,7 @@
         <v>7</v>
       </c>
       <c r="G27" s="8"/>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1503,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="5"/>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1524,7 +2442,7 @@
       <c r="F29" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1545,7 +2463,7 @@
       <c r="F30" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1566,7 +2484,7 @@
       <c r="F31" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1587,7 +2505,7 @@
       <c r="F32" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="21" t="s">
+      <c r="H32" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1609,7 +2527,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="5"/>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1631,7 +2549,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="8"/>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="19" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>